<commit_message>
cierre  12 Nov 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE  HERRADURA  NOVIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE  HERRADURA  NOVIEMBRE   2021.xlsx
@@ -2590,57 +2590,6 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2696,6 +2645,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4311,23 +4311,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="230"/>
-      <c r="C1" s="239" t="s">
+      <c r="B1" s="249"/>
+      <c r="C1" s="258" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -4337,17 +4337,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="232" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="233"/>
+      <c r="B3" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="252"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="253"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -4363,14 +4363,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="235" t="s">
+      <c r="E4" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="236"/>
-      <c r="H4" s="237" t="s">
+      <c r="F4" s="255"/>
+      <c r="H4" s="256" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="238"/>
+      <c r="I4" s="257"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -4380,10 +4380,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="225"/>
+      <c r="Q4" s="244"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -5878,11 +5878,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="226">
+      <c r="M39" s="245">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="228">
+      <c r="N39" s="247">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -5914,8 +5914,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="227"/>
-      <c r="N40" s="229"/>
+      <c r="M40" s="246"/>
+      <c r="N40" s="248"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -6148,29 +6148,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="250" t="s">
+      <c r="H52" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="251"/>
+      <c r="I52" s="234"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="252">
+      <c r="K52" s="235">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="253"/>
-      <c r="M52" s="241">
+      <c r="L52" s="236"/>
+      <c r="M52" s="224">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="242"/>
+      <c r="N52" s="225"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="254" t="s">
+      <c r="D53" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="254"/>
+      <c r="E53" s="237"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -6181,22 +6181,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="255" t="s">
+      <c r="D54" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="255"/>
+      <c r="E54" s="238"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="256" t="s">
+      <c r="I54" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="257"/>
-      <c r="K54" s="258">
+      <c r="J54" s="240"/>
+      <c r="K54" s="241">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="259"/>
+      <c r="L54" s="242"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6227,10 +6227,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="243">
-        <v>0</v>
-      </c>
-      <c r="L56" s="244"/>
+      <c r="K56" s="226">
+        <v>0</v>
+      </c>
+      <c r="L56" s="227"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -6247,22 +6247,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="245" t="s">
+      <c r="D58" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="246"/>
+      <c r="E58" s="229"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="247" t="s">
+      <c r="I58" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="248"/>
-      <c r="K58" s="249">
+      <c r="J58" s="231"/>
+      <c r="K58" s="232">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="249"/>
+      <c r="L58" s="232"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -6406,6 +6406,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -6417,15 +6426,6 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8139,23 +8139,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="230"/>
-      <c r="C1" s="239" t="s">
+      <c r="B1" s="249"/>
+      <c r="C1" s="258" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -8165,17 +8165,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="232" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="233"/>
+      <c r="B3" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="252"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="253"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -8191,14 +8191,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="235" t="s">
+      <c r="E4" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="236"/>
-      <c r="H4" s="237" t="s">
+      <c r="F4" s="255"/>
+      <c r="H4" s="256" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="238"/>
+      <c r="I4" s="257"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -8208,10 +8208,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="225"/>
+      <c r="Q4" s="244"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -9701,11 +9701,11 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="226">
+      <c r="M39" s="245">
         <f>SUM(M5:M38)</f>
         <v>1464441</v>
       </c>
-      <c r="N39" s="228">
+      <c r="N39" s="247">
         <f>SUM(N5:N38)</f>
         <v>53494</v>
       </c>
@@ -9731,8 +9731,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="227"/>
-      <c r="N40" s="229"/>
+      <c r="M40" s="246"/>
+      <c r="N40" s="248"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -9947,29 +9947,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="250" t="s">
+      <c r="H52" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="251"/>
+      <c r="I52" s="234"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="252">
+      <c r="K52" s="235">
         <f>I50+L50</f>
         <v>69642.26999999999</v>
       </c>
-      <c r="L52" s="253"/>
-      <c r="M52" s="241">
+      <c r="L52" s="236"/>
+      <c r="M52" s="224">
         <f>N39+M39</f>
         <v>1517935</v>
       </c>
-      <c r="N52" s="242"/>
+      <c r="N52" s="225"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="254" t="s">
+      <c r="D53" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="254"/>
+      <c r="E53" s="237"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1505921.23</v>
@@ -9980,22 +9980,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="255" t="s">
+      <c r="D54" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="255"/>
+      <c r="E54" s="238"/>
       <c r="F54" s="102">
         <v>-1424333.95</v>
       </c>
-      <c r="I54" s="256" t="s">
+      <c r="I54" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="257"/>
-      <c r="K54" s="258">
+      <c r="J54" s="240"/>
+      <c r="K54" s="241">
         <f>F56+F57+F58</f>
         <v>222140.17000000004</v>
       </c>
-      <c r="L54" s="259"/>
+      <c r="L54" s="242"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -10026,11 +10026,11 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="243">
+      <c r="K56" s="226">
         <f>-C4</f>
         <v>-136234.76999999999</v>
       </c>
-      <c r="L56" s="244"/>
+      <c r="L56" s="227"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -10047,22 +10047,22 @@
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="245" t="s">
+      <c r="D58" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="246"/>
+      <c r="E58" s="229"/>
       <c r="F58" s="121">
         <v>134848.89000000001</v>
       </c>
-      <c r="I58" s="247" t="s">
+      <c r="I58" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="248"/>
-      <c r="K58" s="249">
+      <c r="J58" s="231"/>
+      <c r="K58" s="232">
         <f>K54+K56</f>
         <v>85905.400000000052</v>
       </c>
-      <c r="L58" s="249"/>
+      <c r="L58" s="232"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -10206,6 +10206,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -10220,12 +10226,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11826,8 +11826,8 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11849,23 +11849,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="230"/>
-      <c r="C1" s="239" t="s">
+      <c r="B1" s="249"/>
+      <c r="C1" s="258" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -11875,17 +11875,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="232" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="233"/>
+      <c r="B3" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="252"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="253"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -11901,14 +11901,14 @@
       <c r="D4" s="16">
         <v>44472</v>
       </c>
-      <c r="E4" s="235" t="s">
+      <c r="E4" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="236"/>
-      <c r="H4" s="237" t="s">
+      <c r="F4" s="255"/>
+      <c r="H4" s="256" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="238"/>
+      <c r="I4" s="257"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -11918,10 +11918,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="225"/>
+      <c r="Q4" s="244"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -13496,11 +13496,11 @@
       <c r="L40" s="69">
         <v>1195.68</v>
       </c>
-      <c r="M40" s="226">
+      <c r="M40" s="245">
         <f>SUM(M5:M39)</f>
         <v>1982944.5</v>
       </c>
-      <c r="N40" s="228">
+      <c r="N40" s="247">
         <f>SUM(N5:N39)</f>
         <v>62048</v>
       </c>
@@ -13530,10 +13530,10 @@
         <v>265</v>
       </c>
       <c r="L41" s="69">
-        <v>738.22</v>
-      </c>
-      <c r="M41" s="227"/>
-      <c r="N41" s="229"/>
+        <v>942.84</v>
+      </c>
+      <c r="M41" s="246"/>
+      <c r="N41" s="248"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -13748,7 +13748,7 @@
       </c>
       <c r="L51" s="101">
         <f>SUM(L5:L50)</f>
-        <v>102006.04999999999</v>
+        <v>102210.66999999998</v>
       </c>
       <c r="M51" s="102"/>
       <c r="N51" s="102"/>
@@ -13766,32 +13766,32 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="250" t="s">
+      <c r="H53" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="251"/>
+      <c r="I53" s="234"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="252">
+      <c r="K53" s="235">
         <f>I51+L51</f>
-        <v>103934.54999999999</v>
-      </c>
-      <c r="L53" s="253"/>
-      <c r="M53" s="241">
+        <v>104139.16999999998</v>
+      </c>
+      <c r="L53" s="236"/>
+      <c r="M53" s="224">
         <f>N40+M40</f>
         <v>2044992.5</v>
       </c>
-      <c r="N53" s="242"/>
+      <c r="N53" s="225"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="254" t="s">
+      <c r="D54" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="254"/>
+      <c r="E54" s="237"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
-        <v>2004809.95</v>
+        <v>2004605.33</v>
       </c>
       <c r="I54" s="108"/>
       <c r="J54" s="109"/>
@@ -13799,22 +13799,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="255" t="s">
+      <c r="D55" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="255"/>
+      <c r="E55" s="238"/>
       <c r="F55" s="102">
         <v>-2026393.17</v>
       </c>
-      <c r="I55" s="256" t="s">
+      <c r="I55" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="257"/>
-      <c r="K55" s="258">
+      <c r="J55" s="240"/>
+      <c r="K55" s="241">
         <f>F57+F58+F59</f>
-        <v>178916.18000000002</v>
-      </c>
-      <c r="L55" s="259"/>
+        <v>178711.56000000014</v>
+      </c>
+      <c r="L55" s="242"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -13838,18 +13838,18 @@
       </c>
       <c r="F57" s="102">
         <f>SUM(F54:F56)</f>
-        <v>-21583.219999999972</v>
+        <v>-21787.839999999851</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="243">
+      <c r="K57" s="226">
         <f>-C4</f>
         <v>-134848.89000000001</v>
       </c>
-      <c r="L57" s="244"/>
+      <c r="L57" s="227"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -13866,22 +13866,22 @@
       <c r="C59" s="120">
         <v>44507</v>
       </c>
-      <c r="D59" s="245" t="s">
+      <c r="D59" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="246"/>
+      <c r="E59" s="229"/>
       <c r="F59" s="121">
         <v>192529.4</v>
       </c>
-      <c r="I59" s="247" t="s">
+      <c r="I59" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="248"/>
-      <c r="K59" s="249">
+      <c r="J59" s="231"/>
+      <c r="K59" s="232">
         <f>K55+K57</f>
-        <v>44067.290000000008</v>
-      </c>
-      <c r="L59" s="249"/>
+        <v>43862.670000000129</v>
+      </c>
+      <c r="L59" s="232"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -14025,6 +14025,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
@@ -14039,12 +14045,6 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 24 NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE  HERRADURA  NOVIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE  HERRADURA  NOVIEMBRE   2021.xlsx
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="279">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1069,6 +1069,39 @@
   </si>
   <si>
     <t>LONGANIZA</t>
+  </si>
+  <si>
+    <t>QUESO</t>
+  </si>
+  <si>
+    <t>TOCINO-JAMON-CONDIMENTOS-QUESO-PAN ARABE-RETAZO-</t>
+  </si>
+  <si>
+    <t>CEBOLLA--PEREJIL</t>
+  </si>
+  <si>
+    <t>NOMINA # 46 y vac</t>
+  </si>
+  <si>
+    <t>PAPAS-SANCHICHA-CECINA</t>
+  </si>
+  <si>
+    <t>SALAMI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOCINO   </t>
+  </si>
+  <si>
+    <t>ARABE</t>
+  </si>
+  <si>
+    <t>NOMINA # 47</t>
+  </si>
+  <si>
+    <t>RETAZO--TOCINO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEBOLLA   </t>
   </si>
 </sst>
 </file>
@@ -2656,57 +2689,6 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2762,6 +2744,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4803,23 +4836,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="230"/>
-      <c r="C1" s="239" t="s">
+      <c r="B1" s="249"/>
+      <c r="C1" s="258" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -4829,17 +4862,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="232" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="233"/>
+      <c r="B3" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="252"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="253"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -4855,14 +4888,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="235" t="s">
+      <c r="E4" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="236"/>
-      <c r="H4" s="237" t="s">
+      <c r="F4" s="255"/>
+      <c r="H4" s="256" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="238"/>
+      <c r="I4" s="257"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -4872,10 +4905,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="225"/>
+      <c r="Q4" s="244"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -6370,11 +6403,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="226">
+      <c r="M39" s="245">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="228">
+      <c r="N39" s="247">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -6406,8 +6439,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="227"/>
-      <c r="N40" s="229"/>
+      <c r="M40" s="246"/>
+      <c r="N40" s="248"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -6640,29 +6673,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="250" t="s">
+      <c r="H52" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="251"/>
+      <c r="I52" s="234"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="252">
+      <c r="K52" s="235">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="253"/>
-      <c r="M52" s="241">
+      <c r="L52" s="236"/>
+      <c r="M52" s="224">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="242"/>
+      <c r="N52" s="225"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="254" t="s">
+      <c r="D53" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="254"/>
+      <c r="E53" s="237"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -6673,22 +6706,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="255" t="s">
+      <c r="D54" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="255"/>
+      <c r="E54" s="238"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="256" t="s">
+      <c r="I54" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="257"/>
-      <c r="K54" s="258">
+      <c r="J54" s="240"/>
+      <c r="K54" s="241">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="259"/>
+      <c r="L54" s="242"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6719,10 +6752,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="243">
-        <v>0</v>
-      </c>
-      <c r="L56" s="244"/>
+      <c r="K56" s="226">
+        <v>0</v>
+      </c>
+      <c r="L56" s="227"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -6739,22 +6772,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="245" t="s">
+      <c r="D58" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="246"/>
+      <c r="E58" s="229"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="247" t="s">
+      <c r="I58" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="248"/>
-      <c r="K58" s="249">
+      <c r="J58" s="231"/>
+      <c r="K58" s="232">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="249"/>
+      <c r="L58" s="232"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -6898,6 +6931,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -6909,15 +6951,6 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8829,23 +8862,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="230"/>
-      <c r="C1" s="239" t="s">
+      <c r="B1" s="249"/>
+      <c r="C1" s="258" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -8855,17 +8888,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="232" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="233"/>
+      <c r="B3" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="252"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="253"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -8881,14 +8914,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="235" t="s">
+      <c r="E4" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="236"/>
-      <c r="H4" s="237" t="s">
+      <c r="F4" s="255"/>
+      <c r="H4" s="256" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="238"/>
+      <c r="I4" s="257"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -8898,10 +8931,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="225"/>
+      <c r="Q4" s="244"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -10391,11 +10424,11 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="226">
+      <c r="M39" s="245">
         <f>SUM(M5:M38)</f>
         <v>1464441</v>
       </c>
-      <c r="N39" s="228">
+      <c r="N39" s="247">
         <f>SUM(N5:N38)</f>
         <v>53494</v>
       </c>
@@ -10421,8 +10454,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="227"/>
-      <c r="N40" s="229"/>
+      <c r="M40" s="246"/>
+      <c r="N40" s="248"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -10637,29 +10670,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="250" t="s">
+      <c r="H52" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="251"/>
+      <c r="I52" s="234"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="252">
+      <c r="K52" s="235">
         <f>I50+L50</f>
         <v>69642.26999999999</v>
       </c>
-      <c r="L52" s="253"/>
-      <c r="M52" s="241">
+      <c r="L52" s="236"/>
+      <c r="M52" s="224">
         <f>N39+M39</f>
         <v>1517935</v>
       </c>
-      <c r="N52" s="242"/>
+      <c r="N52" s="225"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="254" t="s">
+      <c r="D53" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="254"/>
+      <c r="E53" s="237"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1505921.23</v>
@@ -10670,22 +10703,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="255" t="s">
+      <c r="D54" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="255"/>
+      <c r="E54" s="238"/>
       <c r="F54" s="102">
         <v>-1424333.95</v>
       </c>
-      <c r="I54" s="256" t="s">
+      <c r="I54" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="257"/>
-      <c r="K54" s="258">
+      <c r="J54" s="240"/>
+      <c r="K54" s="241">
         <f>F56+F57+F58</f>
         <v>222140.17000000004</v>
       </c>
-      <c r="L54" s="259"/>
+      <c r="L54" s="242"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -10716,11 +10749,11 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="243">
+      <c r="K56" s="226">
         <f>-C4</f>
         <v>-136234.76999999999</v>
       </c>
-      <c r="L56" s="244"/>
+      <c r="L56" s="227"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -10737,22 +10770,22 @@
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="245" t="s">
+      <c r="D58" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="246"/>
+      <c r="E58" s="229"/>
       <c r="F58" s="121">
         <v>134848.89000000001</v>
       </c>
-      <c r="I58" s="247" t="s">
+      <c r="I58" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="248"/>
-      <c r="K58" s="249">
+      <c r="J58" s="231"/>
+      <c r="K58" s="232">
         <f>K54+K56</f>
         <v>85905.400000000052</v>
       </c>
-      <c r="L58" s="249"/>
+      <c r="L58" s="232"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -10896,6 +10929,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -10910,12 +10949,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12539,23 +12572,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="230"/>
-      <c r="C1" s="239" t="s">
+      <c r="B1" s="249"/>
+      <c r="C1" s="258" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -12565,17 +12598,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="232" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="233"/>
+      <c r="B3" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="252"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="253"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -12591,14 +12624,14 @@
       <c r="D4" s="16">
         <v>44472</v>
       </c>
-      <c r="E4" s="235" t="s">
+      <c r="E4" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="236"/>
-      <c r="H4" s="237" t="s">
+      <c r="F4" s="255"/>
+      <c r="H4" s="256" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="238"/>
+      <c r="I4" s="257"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -12608,10 +12641,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="225"/>
+      <c r="Q4" s="244"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -14186,11 +14219,11 @@
       <c r="L40" s="69">
         <v>1195.68</v>
       </c>
-      <c r="M40" s="226">
+      <c r="M40" s="245">
         <f>SUM(M5:M39)</f>
         <v>1982944.5</v>
       </c>
-      <c r="N40" s="228">
+      <c r="N40" s="247">
         <f>SUM(N5:N39)</f>
         <v>62048</v>
       </c>
@@ -14222,8 +14255,8 @@
       <c r="L41" s="69">
         <v>942.84</v>
       </c>
-      <c r="M41" s="227"/>
-      <c r="N41" s="229"/>
+      <c r="M41" s="246"/>
+      <c r="N41" s="248"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -14456,29 +14489,29 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="250" t="s">
+      <c r="H53" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="251"/>
+      <c r="I53" s="234"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="252">
+      <c r="K53" s="235">
         <f>I51+L51</f>
         <v>104139.16999999998</v>
       </c>
-      <c r="L53" s="253"/>
-      <c r="M53" s="241">
+      <c r="L53" s="236"/>
+      <c r="M53" s="224">
         <f>N40+M40</f>
         <v>2044992.5</v>
       </c>
-      <c r="N53" s="242"/>
+      <c r="N53" s="225"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="254" t="s">
+      <c r="D54" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="254"/>
+      <c r="E54" s="237"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
         <v>2004605.33</v>
@@ -14489,22 +14522,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="255" t="s">
+      <c r="D55" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="255"/>
+      <c r="E55" s="238"/>
       <c r="F55" s="102">
         <v>-2026393.17</v>
       </c>
-      <c r="I55" s="256" t="s">
+      <c r="I55" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="257"/>
-      <c r="K55" s="258">
+      <c r="J55" s="240"/>
+      <c r="K55" s="241">
         <f>F57+F58+F59</f>
         <v>178711.56000000014</v>
       </c>
-      <c r="L55" s="259"/>
+      <c r="L55" s="242"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -14535,11 +14568,11 @@
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="243">
+      <c r="K57" s="226">
         <f>-C4</f>
         <v>-134848.89000000001</v>
       </c>
-      <c r="L57" s="244"/>
+      <c r="L57" s="227"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -14556,22 +14589,22 @@
       <c r="C59" s="120">
         <v>44507</v>
       </c>
-      <c r="D59" s="245" t="s">
+      <c r="D59" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="246"/>
+      <c r="E59" s="229"/>
       <c r="F59" s="121">
         <v>192529.4</v>
       </c>
-      <c r="I59" s="247" t="s">
+      <c r="I59" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="248"/>
-      <c r="K59" s="249">
+      <c r="J59" s="231"/>
+      <c r="K59" s="232">
         <f>K55+K57</f>
         <v>43862.670000000129</v>
       </c>
-      <c r="L59" s="249"/>
+      <c r="L59" s="232"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -14715,6 +14748,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
@@ -14729,12 +14768,6 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16429,8 +16462,8 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16452,23 +16485,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="230"/>
-      <c r="C1" s="239" t="s">
+      <c r="B1" s="249"/>
+      <c r="C1" s="258" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -16478,17 +16511,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="232" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="233"/>
+      <c r="B3" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="252"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="253"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -16504,14 +16537,14 @@
       <c r="D4" s="16">
         <v>44507</v>
       </c>
-      <c r="E4" s="235" t="s">
+      <c r="E4" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="236"/>
-      <c r="H4" s="237" t="s">
+      <c r="F4" s="255"/>
+      <c r="H4" s="256" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="238"/>
+      <c r="I4" s="257"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -16521,10 +16554,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="225"/>
+      <c r="Q4" s="244"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -16619,34 +16652,43 @@
       <c r="B7" s="21">
         <v>44510</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="22">
+        <v>80</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>268</v>
+      </c>
       <c r="E7" s="24">
         <v>44510</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="25">
+        <v>28829</v>
+      </c>
       <c r="G7" s="26"/>
       <c r="H7" s="32">
         <v>44510</v>
       </c>
-      <c r="I7" s="28"/>
+      <c r="I7" s="28">
+        <v>33</v>
+      </c>
       <c r="J7" s="33"/>
       <c r="K7" s="37"/>
       <c r="L7" s="35"/>
       <c r="M7" s="138">
-        <v>0</v>
+        <f>22800+5000</f>
+        <v>27800</v>
       </c>
       <c r="N7" s="30">
-        <v>0</v>
+        <v>917</v>
       </c>
       <c r="O7" s="26"/>
       <c r="P7" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28830</v>
       </c>
       <c r="Q7" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="26"/>
     </row>
@@ -16655,22 +16697,30 @@
       <c r="B8" s="21">
         <v>44511</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="22">
+        <v>19923</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>269</v>
+      </c>
       <c r="E8" s="24">
         <v>44511</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="25">
+        <v>49002</v>
+      </c>
       <c r="G8" s="26"/>
       <c r="H8" s="32">
         <v>44511</v>
       </c>
-      <c r="I8" s="28"/>
+      <c r="I8" s="28">
+        <v>11</v>
+      </c>
       <c r="J8" s="39"/>
       <c r="K8" s="40"/>
       <c r="L8" s="35"/>
       <c r="M8" s="138">
-        <v>0</v>
+        <v>29070</v>
       </c>
       <c r="N8" s="30">
         <v>0</v>
@@ -16678,11 +16728,11 @@
       <c r="O8" s="26"/>
       <c r="P8" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>49004</v>
       </c>
       <c r="Q8" s="76">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R8" s="51"/>
     </row>
@@ -16691,34 +16741,43 @@
       <c r="B9" s="21">
         <v>44512</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="22">
+        <v>3480</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>200</v>
+      </c>
       <c r="E9" s="24">
         <v>44512</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="25">
+        <v>78448</v>
+      </c>
       <c r="G9" s="26"/>
       <c r="H9" s="32">
         <v>44512</v>
       </c>
-      <c r="I9" s="28"/>
+      <c r="I9" s="28">
+        <v>1659</v>
+      </c>
       <c r="J9" s="33"/>
       <c r="K9" s="41"/>
       <c r="L9" s="35"/>
       <c r="M9" s="138">
-        <v>0</v>
+        <f>25000+47260</f>
+        <v>72260</v>
       </c>
       <c r="N9" s="30">
-        <v>0</v>
+        <v>1050</v>
       </c>
       <c r="O9" s="26"/>
       <c r="P9" s="83">
         <f>N9+M9+L9+I9+C9</f>
-        <v>0</v>
+        <v>78449</v>
       </c>
       <c r="Q9" s="9">
         <f>P9-F9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="26"/>
     </row>
@@ -16727,34 +16786,50 @@
       <c r="B10" s="21">
         <v>44513</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="31"/>
+      <c r="C10" s="22">
+        <v>19</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>270</v>
+      </c>
       <c r="E10" s="24">
         <v>44513</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="25">
+        <v>77465</v>
+      </c>
       <c r="G10" s="26"/>
       <c r="H10" s="32">
         <v>44513</v>
       </c>
-      <c r="I10" s="28"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43"/>
+      <c r="I10" s="28">
+        <v>129</v>
+      </c>
+      <c r="J10" s="33">
+        <v>44513</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="L10" s="43">
+        <f>10814.29+1285.71</f>
+        <v>12100</v>
+      </c>
       <c r="M10" s="138">
-        <v>0</v>
+        <f>30000+29340</f>
+        <v>59340</v>
       </c>
       <c r="N10" s="30">
-        <v>0</v>
+        <v>5875</v>
       </c>
       <c r="O10" s="26"/>
       <c r="P10" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>77463</v>
+      </c>
+      <c r="Q10" s="217">
+        <f t="shared" si="1"/>
+        <v>-2</v>
       </c>
       <c r="R10" s="51"/>
     </row>
@@ -16763,34 +16838,43 @@
       <c r="B11" s="21">
         <v>44514</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="31"/>
+      <c r="C11" s="22">
+        <v>962</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>272</v>
+      </c>
       <c r="E11" s="24">
         <v>44514</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="25">
+        <v>94524</v>
+      </c>
       <c r="G11" s="26"/>
       <c r="H11" s="32">
         <v>44514</v>
       </c>
-      <c r="I11" s="28"/>
+      <c r="I11" s="28">
+        <v>3010</v>
+      </c>
       <c r="J11" s="39"/>
       <c r="K11" s="44"/>
       <c r="L11" s="35"/>
       <c r="M11" s="138">
-        <v>0</v>
+        <f>75000+13050</f>
+        <v>88050</v>
       </c>
       <c r="N11" s="30">
-        <v>0</v>
+        <v>2494</v>
       </c>
       <c r="O11" s="26"/>
       <c r="P11" s="83">
         <f>N11+M11+L11+I11+C11</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>94516</v>
+      </c>
+      <c r="Q11" s="217">
+        <f t="shared" si="1"/>
+        <v>-8</v>
       </c>
       <c r="R11" s="26"/>
     </row>
@@ -16799,30 +16883,37 @@
       <c r="B12" s="21">
         <v>44515</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="22">
+        <v>0</v>
+      </c>
       <c r="D12" s="31"/>
       <c r="E12" s="24">
         <v>44515</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="25">
+        <v>60081</v>
+      </c>
       <c r="G12" s="26"/>
       <c r="H12" s="32">
         <v>44515</v>
       </c>
-      <c r="I12" s="28"/>
+      <c r="I12" s="28">
+        <v>88</v>
+      </c>
       <c r="J12" s="33"/>
       <c r="K12" s="45"/>
       <c r="L12" s="35"/>
       <c r="M12" s="138">
-        <v>0</v>
+        <f>30000+29410</f>
+        <v>59410</v>
       </c>
       <c r="N12" s="30">
-        <v>0</v>
+        <v>583</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60081</v>
       </c>
       <c r="Q12" s="9">
         <f t="shared" si="1"/>
@@ -16835,34 +16926,43 @@
       <c r="B13" s="21">
         <v>44516</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="22">
+        <v>1738</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>273</v>
+      </c>
       <c r="E13" s="24">
         <v>44516</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="25">
+        <v>47537</v>
+      </c>
       <c r="G13" s="26"/>
       <c r="H13" s="32">
         <v>44516</v>
       </c>
-      <c r="I13" s="28"/>
+      <c r="I13" s="28">
+        <v>15</v>
+      </c>
       <c r="J13" s="33"/>
       <c r="K13" s="46"/>
       <c r="L13" s="35"/>
       <c r="M13" s="138">
-        <v>0</v>
+        <f>20000+25440</f>
+        <v>45440</v>
       </c>
       <c r="N13" s="30">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="O13" s="26"/>
       <c r="P13" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47541</v>
       </c>
       <c r="Q13" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R13" s="204"/>
     </row>
@@ -16871,34 +16971,42 @@
       <c r="B14" s="21">
         <v>44517</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="36"/>
+      <c r="C14" s="22">
+        <v>4190</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>200</v>
+      </c>
       <c r="E14" s="24">
         <v>44517</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="25">
+        <v>51862</v>
+      </c>
       <c r="G14" s="26"/>
       <c r="H14" s="32">
         <v>44517</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="28">
+        <v>40</v>
+      </c>
       <c r="J14" s="33"/>
       <c r="K14" s="40"/>
       <c r="L14" s="35"/>
       <c r="M14" s="138">
-        <v>0</v>
+        <v>45290</v>
       </c>
       <c r="N14" s="30">
-        <v>0</v>
+        <v>2345</v>
       </c>
       <c r="O14" s="26"/>
       <c r="P14" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>51865</v>
       </c>
       <c r="Q14" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R14" s="204"/>
     </row>
@@ -16907,33 +17015,40 @@
       <c r="B15" s="21">
         <v>44518</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="22">
+        <v>0</v>
+      </c>
       <c r="D15" s="36"/>
       <c r="E15" s="24">
         <v>44518</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="25">
+        <v>68774</v>
+      </c>
       <c r="G15" s="26"/>
       <c r="H15" s="32">
         <v>44518</v>
       </c>
-      <c r="I15" s="28"/>
+      <c r="I15" s="28">
+        <v>15</v>
+      </c>
       <c r="J15" s="33"/>
       <c r="K15" s="40"/>
       <c r="L15" s="35"/>
       <c r="M15" s="138">
-        <v>0</v>
+        <f>500+43260+25000</f>
+        <v>68760</v>
       </c>
       <c r="N15" s="30">
         <v>0</v>
       </c>
       <c r="P15" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="217">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>68775</v>
+      </c>
+      <c r="Q15" s="136">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R15" s="26"/>
     </row>
@@ -16942,33 +17057,42 @@
       <c r="B16" s="21">
         <v>44519</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="31"/>
+      <c r="C16" s="22">
+        <v>752</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>274</v>
+      </c>
       <c r="E16" s="24">
         <v>44519</v>
       </c>
-      <c r="F16" s="25"/>
+      <c r="F16" s="25">
+        <v>71014</v>
+      </c>
       <c r="G16" s="26"/>
       <c r="H16" s="32">
         <v>44519</v>
       </c>
-      <c r="I16" s="28"/>
+      <c r="I16" s="28">
+        <v>40</v>
+      </c>
       <c r="J16" s="33"/>
       <c r="K16" s="40"/>
       <c r="L16" s="9"/>
       <c r="M16" s="138">
-        <v>0</v>
+        <f>30000+39840</f>
+        <v>69840</v>
       </c>
       <c r="N16" s="30">
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="P16" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71017</v>
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R16" s="26"/>
     </row>
@@ -16977,33 +17101,48 @@
       <c r="B17" s="21">
         <v>44520</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="22">
+        <v>23</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>275</v>
+      </c>
       <c r="E17" s="24">
         <v>44520</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="25">
+        <v>70966</v>
+      </c>
       <c r="G17" s="26"/>
       <c r="H17" s="32">
         <v>44520</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="43"/>
+      <c r="I17" s="28">
+        <v>73</v>
+      </c>
+      <c r="J17" s="33">
+        <v>44520</v>
+      </c>
+      <c r="K17" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="L17" s="43">
+        <v>13341.34</v>
+      </c>
       <c r="M17" s="138">
-        <v>0</v>
+        <f>30000+22220</f>
+        <v>52220</v>
       </c>
       <c r="N17" s="30">
-        <v>0</v>
+        <v>5300</v>
       </c>
       <c r="P17" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70957.34</v>
+      </c>
+      <c r="Q17" s="217">
+        <f t="shared" si="1"/>
+        <v>-8.6600000000034925</v>
       </c>
       <c r="R17" s="26"/>
     </row>
@@ -17012,33 +17151,42 @@
       <c r="B18" s="21">
         <v>44521</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="31"/>
+      <c r="C18" s="22">
+        <v>3983</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>277</v>
+      </c>
       <c r="E18" s="24">
         <v>44521</v>
       </c>
-      <c r="F18" s="25"/>
+      <c r="F18" s="25">
+        <v>152652</v>
+      </c>
       <c r="G18" s="26"/>
       <c r="H18" s="32">
         <v>44521</v>
       </c>
-      <c r="I18" s="28"/>
+      <c r="I18" s="28">
+        <v>0</v>
+      </c>
       <c r="J18" s="33"/>
       <c r="K18" s="47"/>
       <c r="L18" s="35"/>
       <c r="M18" s="138">
-        <v>0</v>
+        <f>70000+60000+17770</f>
+        <v>147770</v>
       </c>
       <c r="N18" s="30">
-        <v>0</v>
+        <v>903</v>
       </c>
       <c r="P18" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>152656</v>
       </c>
       <c r="Q18" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R18" s="26"/>
     </row>
@@ -17047,33 +17195,42 @@
       <c r="B19" s="21">
         <v>44522</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="22">
+        <v>14</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>278</v>
+      </c>
       <c r="E19" s="24">
         <v>44522</v>
       </c>
-      <c r="F19" s="25"/>
+      <c r="F19" s="25">
+        <v>47787</v>
+      </c>
       <c r="G19" s="26"/>
       <c r="H19" s="32">
         <v>44522</v>
       </c>
-      <c r="I19" s="28"/>
+      <c r="I19" s="28">
+        <v>45</v>
+      </c>
       <c r="J19" s="33"/>
       <c r="K19" s="48"/>
       <c r="L19" s="49"/>
       <c r="M19" s="138">
-        <v>0</v>
+        <f>25000+22350</f>
+        <v>47350</v>
       </c>
       <c r="N19" s="30">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="P19" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47792</v>
       </c>
       <c r="Q19" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R19" s="26"/>
     </row>
@@ -17747,21 +17904,21 @@
       <c r="J40" s="67"/>
       <c r="K40" s="82"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="226">
+      <c r="M40" s="245">
         <f>SUM(M5:M39)</f>
-        <v>94358</v>
-      </c>
-      <c r="N40" s="228">
+        <v>906958</v>
+      </c>
+      <c r="N40" s="247">
         <f>SUM(N5:N39)</f>
-        <v>0</v>
+        <v>20583</v>
       </c>
       <c r="P40" s="83">
         <f>SUM(P5:P39)</f>
-        <v>97625</v>
+        <v>996571.34</v>
       </c>
       <c r="Q40" s="222">
         <f>SUM(Q5:Q38)</f>
-        <v>7994</v>
+        <v>7999.3399999999965</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17777,8 +17934,8 @@
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="69"/>
-      <c r="M41" s="227"/>
-      <c r="N41" s="229"/>
+      <c r="M41" s="246"/>
+      <c r="N41" s="248"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -17951,7 +18108,7 @@
       </c>
       <c r="C51" s="93">
         <f>SUM(C5:C50)</f>
-        <v>2720</v>
+        <v>37884</v>
       </c>
       <c r="D51" s="94"/>
       <c r="E51" s="95" t="s">
@@ -17959,7 +18116,7 @@
       </c>
       <c r="F51" s="96">
         <f>SUM(F5:F50)</f>
-        <v>89631</v>
+        <v>988572</v>
       </c>
       <c r="G51" s="94"/>
       <c r="H51" s="97" t="s">
@@ -17967,7 +18124,7 @@
       </c>
       <c r="I51" s="98">
         <f>SUM(I5:I50)</f>
-        <v>547</v>
+        <v>5705</v>
       </c>
       <c r="J51" s="99"/>
       <c r="K51" s="100" t="s">
@@ -17975,7 +18132,7 @@
       </c>
       <c r="L51" s="101">
         <f>SUM(L5:L50)</f>
-        <v>0</v>
+        <v>25441.34</v>
       </c>
       <c r="M51" s="102"/>
       <c r="N51" s="102"/>
@@ -17993,32 +18150,32 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="250" t="s">
+      <c r="H53" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="251"/>
+      <c r="I53" s="234"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="252">
+      <c r="K53" s="235">
         <f>I51+L51</f>
-        <v>547</v>
-      </c>
-      <c r="L53" s="253"/>
-      <c r="M53" s="241">
+        <v>31146.34</v>
+      </c>
+      <c r="L53" s="236"/>
+      <c r="M53" s="224">
         <f>N40+M40</f>
-        <v>94358</v>
-      </c>
-      <c r="N53" s="242"/>
+        <v>927541</v>
+      </c>
+      <c r="N53" s="225"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="254" t="s">
+      <c r="D54" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="254"/>
+      <c r="E54" s="237"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
-        <v>86364</v>
+        <v>919541.66</v>
       </c>
       <c r="I54" s="108"/>
       <c r="J54" s="109"/>
@@ -18026,22 +18183,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="255" t="s">
+      <c r="D55" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="255"/>
+      <c r="E55" s="238"/>
       <c r="F55" s="102">
         <v>0</v>
       </c>
-      <c r="I55" s="256" t="s">
+      <c r="I55" s="239" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="257"/>
-      <c r="K55" s="258">
+      <c r="J55" s="240"/>
+      <c r="K55" s="241">
         <f>F57+F58+F59</f>
-        <v>86364</v>
-      </c>
-      <c r="L55" s="259"/>
+        <v>919541.66</v>
+      </c>
+      <c r="L55" s="242"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -18065,18 +18222,18 @@
       </c>
       <c r="F57" s="102">
         <f>SUM(F54:F56)</f>
-        <v>86364</v>
+        <v>919541.66</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="243">
+      <c r="K57" s="226">
         <f>-C4</f>
         <v>-192529.4</v>
       </c>
-      <c r="L57" s="244"/>
+      <c r="L57" s="227"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -18091,22 +18248,22 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="120"/>
-      <c r="D59" s="245" t="s">
+      <c r="D59" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="246"/>
+      <c r="E59" s="229"/>
       <c r="F59" s="121">
         <v>0</v>
       </c>
-      <c r="I59" s="247" t="s">
+      <c r="I59" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="248"/>
-      <c r="K59" s="249">
+      <c r="J59" s="231"/>
+      <c r="K59" s="232">
         <f>K55+K57</f>
-        <v>-106165.4</v>
-      </c>
-      <c r="L59" s="249"/>
+        <v>727012.26</v>
+      </c>
+      <c r="L59" s="232"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -18250,11 +18407,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
@@ -18264,12 +18422,11 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.15748031496062992" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 26 Nov 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE  HERRADURA  NOVIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE  HERRADURA  NOVIEMBRE   2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="A G O S T O    2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="293">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1102,6 +1102,48 @@
   </si>
   <si>
     <t xml:space="preserve">CEBOLLA   </t>
+  </si>
+  <si>
+    <t>00972 C</t>
+  </si>
+  <si>
+    <t>01243 C</t>
+  </si>
+  <si>
+    <t>01245 C</t>
+  </si>
+  <si>
+    <t>01256 C</t>
+  </si>
+  <si>
+    <t>01328 C</t>
+  </si>
+  <si>
+    <t>01540 C</t>
+  </si>
+  <si>
+    <t>01556 C</t>
+  </si>
+  <si>
+    <t>01597 C</t>
+  </si>
+  <si>
+    <t>01626 C</t>
+  </si>
+  <si>
+    <t>01761 C</t>
+  </si>
+  <si>
+    <t>01781 C</t>
+  </si>
+  <si>
+    <t>01976 C</t>
+  </si>
+  <si>
+    <t>01977 C</t>
+  </si>
+  <si>
+    <t>02046 C</t>
   </si>
 </sst>
 </file>
@@ -2266,7 +2308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="266">
+  <cellXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -2689,6 +2731,7 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="17" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2824,9 +2867,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFF6600"/>
       <color rgb="FF33CCFF"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FF9933FF"/>
     </mruColors>
   </colors>
@@ -4836,23 +4879,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="249"/>
-      <c r="C1" s="258" t="s">
+      <c r="B1" s="250"/>
+      <c r="C1" s="259" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="259"/>
-      <c r="L1" s="259"/>
-      <c r="M1" s="259"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="260"/>
+      <c r="F1" s="260"/>
+      <c r="G1" s="260"/>
+      <c r="H1" s="260"/>
+      <c r="I1" s="260"/>
+      <c r="J1" s="260"/>
+      <c r="K1" s="260"/>
+      <c r="L1" s="260"/>
+      <c r="M1" s="260"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="250"/>
+      <c r="B2" s="251"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -4862,17 +4905,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="251" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="252"/>
+      <c r="B3" s="252" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="253"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="253" t="s">
+      <c r="H3" s="254" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="253"/>
+      <c r="I3" s="254"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -4888,14 +4931,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="254" t="s">
+      <c r="E4" s="255" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="255"/>
-      <c r="H4" s="256" t="s">
+      <c r="F4" s="256"/>
+      <c r="H4" s="257" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="257"/>
+      <c r="I4" s="258"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -4905,10 +4948,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="243" t="s">
+      <c r="P4" s="244" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="244"/>
+      <c r="Q4" s="245"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -6403,11 +6446,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="245">
+      <c r="M39" s="246">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="247">
+      <c r="N39" s="248">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -6439,8 +6482,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="246"/>
-      <c r="N40" s="248"/>
+      <c r="M40" s="247"/>
+      <c r="N40" s="249"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -6673,29 +6716,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="233" t="s">
+      <c r="H52" s="234" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="234"/>
+      <c r="I52" s="235"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="235">
+      <c r="K52" s="236">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="236"/>
-      <c r="M52" s="224">
+      <c r="L52" s="237"/>
+      <c r="M52" s="225">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="225"/>
+      <c r="N52" s="226"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="237" t="s">
+      <c r="D53" s="238" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="237"/>
+      <c r="E53" s="238"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -6706,22 +6749,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="238" t="s">
+      <c r="D54" s="239" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="238"/>
+      <c r="E54" s="239"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="239" t="s">
+      <c r="I54" s="240" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="240"/>
-      <c r="K54" s="241">
+      <c r="J54" s="241"/>
+      <c r="K54" s="242">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="242"/>
+      <c r="L54" s="243"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6752,10 +6795,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="226">
-        <v>0</v>
-      </c>
-      <c r="L56" s="227"/>
+      <c r="K56" s="227">
+        <v>0</v>
+      </c>
+      <c r="L56" s="228"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -6772,22 +6815,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="228" t="s">
+      <c r="D58" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="229"/>
+      <c r="E58" s="230"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="230" t="s">
+      <c r="I58" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="231"/>
-      <c r="K58" s="232">
+      <c r="J58" s="232"/>
+      <c r="K58" s="233">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="232"/>
+      <c r="L58" s="233"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -6988,12 +7031,12 @@
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="163"/>
-      <c r="B45" s="263" t="s">
+      <c r="B45" s="264" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="264"/>
-      <c r="D45" s="264"/>
-      <c r="E45" s="265"/>
+      <c r="C45" s="265"/>
+      <c r="D45" s="265"/>
+      <c r="E45" s="266"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7220,7 +7263,7 @@
       <c r="C3" s="35">
         <v>3015.96</v>
       </c>
-      <c r="D3" s="260" t="s">
+      <c r="D3" s="261" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="9"/>
@@ -7239,7 +7282,7 @@
       <c r="C4" s="35">
         <v>10281</v>
       </c>
-      <c r="D4" s="261"/>
+      <c r="D4" s="262"/>
       <c r="E4" s="180"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
@@ -7257,7 +7300,7 @@
       <c r="C5" s="35">
         <v>12746.2</v>
       </c>
-      <c r="D5" s="261"/>
+      <c r="D5" s="262"/>
       <c r="E5" s="180"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
@@ -7274,7 +7317,7 @@
       <c r="C6" s="35">
         <v>28974.78</v>
       </c>
-      <c r="D6" s="261"/>
+      <c r="D6" s="262"/>
       <c r="E6" s="180"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
@@ -7291,7 +7334,7 @@
       <c r="C7" s="35">
         <v>44758.6</v>
       </c>
-      <c r="D7" s="261"/>
+      <c r="D7" s="262"/>
       <c r="E7" s="180"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
@@ -7308,7 +7351,7 @@
       <c r="C8" s="35">
         <v>12841.78</v>
       </c>
-      <c r="D8" s="261"/>
+      <c r="D8" s="262"/>
       <c r="E8" s="180"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
@@ -7325,7 +7368,7 @@
       <c r="C9" s="35">
         <v>3898.05</v>
       </c>
-      <c r="D9" s="261"/>
+      <c r="D9" s="262"/>
       <c r="E9" s="180"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
@@ -7342,7 +7385,7 @@
       <c r="C10" s="35">
         <v>1429</v>
       </c>
-      <c r="D10" s="262"/>
+      <c r="D10" s="263"/>
       <c r="E10" s="180"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
@@ -8862,23 +8905,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="249"/>
-      <c r="C1" s="258" t="s">
+      <c r="B1" s="250"/>
+      <c r="C1" s="259" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="259"/>
-      <c r="L1" s="259"/>
-      <c r="M1" s="259"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="260"/>
+      <c r="F1" s="260"/>
+      <c r="G1" s="260"/>
+      <c r="H1" s="260"/>
+      <c r="I1" s="260"/>
+      <c r="J1" s="260"/>
+      <c r="K1" s="260"/>
+      <c r="L1" s="260"/>
+      <c r="M1" s="260"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="250"/>
+      <c r="B2" s="251"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -8888,17 +8931,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="251" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="252"/>
+      <c r="B3" s="252" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="253"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="253" t="s">
+      <c r="H3" s="254" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="253"/>
+      <c r="I3" s="254"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -8914,14 +8957,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="254" t="s">
+      <c r="E4" s="255" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="255"/>
-      <c r="H4" s="256" t="s">
+      <c r="F4" s="256"/>
+      <c r="H4" s="257" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="257"/>
+      <c r="I4" s="258"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -8931,10 +8974,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="243" t="s">
+      <c r="P4" s="244" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="244"/>
+      <c r="Q4" s="245"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -10424,11 +10467,11 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="245">
+      <c r="M39" s="246">
         <f>SUM(M5:M38)</f>
         <v>1464441</v>
       </c>
-      <c r="N39" s="247">
+      <c r="N39" s="248">
         <f>SUM(N5:N38)</f>
         <v>53494</v>
       </c>
@@ -10454,8 +10497,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="246"/>
-      <c r="N40" s="248"/>
+      <c r="M40" s="247"/>
+      <c r="N40" s="249"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -10670,29 +10713,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="233" t="s">
+      <c r="H52" s="234" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="234"/>
+      <c r="I52" s="235"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="235">
+      <c r="K52" s="236">
         <f>I50+L50</f>
         <v>69642.26999999999</v>
       </c>
-      <c r="L52" s="236"/>
-      <c r="M52" s="224">
+      <c r="L52" s="237"/>
+      <c r="M52" s="225">
         <f>N39+M39</f>
         <v>1517935</v>
       </c>
-      <c r="N52" s="225"/>
+      <c r="N52" s="226"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="237" t="s">
+      <c r="D53" s="238" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="237"/>
+      <c r="E53" s="238"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1505921.23</v>
@@ -10703,22 +10746,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="238" t="s">
+      <c r="D54" s="239" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="238"/>
+      <c r="E54" s="239"/>
       <c r="F54" s="102">
         <v>-1424333.95</v>
       </c>
-      <c r="I54" s="239" t="s">
+      <c r="I54" s="240" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="240"/>
-      <c r="K54" s="241">
+      <c r="J54" s="241"/>
+      <c r="K54" s="242">
         <f>F56+F57+F58</f>
         <v>222140.17000000004</v>
       </c>
-      <c r="L54" s="242"/>
+      <c r="L54" s="243"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -10749,11 +10792,11 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="226">
+      <c r="K56" s="227">
         <f>-C4</f>
         <v>-136234.76999999999</v>
       </c>
-      <c r="L56" s="227"/>
+      <c r="L56" s="228"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -10770,22 +10813,22 @@
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="228" t="s">
+      <c r="D58" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="229"/>
+      <c r="E58" s="230"/>
       <c r="F58" s="121">
         <v>134848.89000000001</v>
       </c>
-      <c r="I58" s="230" t="s">
+      <c r="I58" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="231"/>
-      <c r="K58" s="232">
+      <c r="J58" s="232"/>
+      <c r="K58" s="233">
         <f>K54+K56</f>
         <v>85905.400000000052</v>
       </c>
-      <c r="L58" s="232"/>
+      <c r="L58" s="233"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -12572,23 +12615,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="249"/>
-      <c r="C1" s="258" t="s">
+      <c r="B1" s="250"/>
+      <c r="C1" s="259" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="259"/>
-      <c r="L1" s="259"/>
-      <c r="M1" s="259"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="260"/>
+      <c r="F1" s="260"/>
+      <c r="G1" s="260"/>
+      <c r="H1" s="260"/>
+      <c r="I1" s="260"/>
+      <c r="J1" s="260"/>
+      <c r="K1" s="260"/>
+      <c r="L1" s="260"/>
+      <c r="M1" s="260"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="250"/>
+      <c r="B2" s="251"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -12598,17 +12641,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="251" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="252"/>
+      <c r="B3" s="252" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="253"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="253" t="s">
+      <c r="H3" s="254" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="253"/>
+      <c r="I3" s="254"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -12624,14 +12667,14 @@
       <c r="D4" s="16">
         <v>44472</v>
       </c>
-      <c r="E4" s="254" t="s">
+      <c r="E4" s="255" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="255"/>
-      <c r="H4" s="256" t="s">
+      <c r="F4" s="256"/>
+      <c r="H4" s="257" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="257"/>
+      <c r="I4" s="258"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -12641,10 +12684,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="243" t="s">
+      <c r="P4" s="244" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="244"/>
+      <c r="Q4" s="245"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -14219,11 +14262,11 @@
       <c r="L40" s="69">
         <v>1195.68</v>
       </c>
-      <c r="M40" s="245">
+      <c r="M40" s="246">
         <f>SUM(M5:M39)</f>
         <v>1982944.5</v>
       </c>
-      <c r="N40" s="247">
+      <c r="N40" s="248">
         <f>SUM(N5:N39)</f>
         <v>62048</v>
       </c>
@@ -14255,8 +14298,8 @@
       <c r="L41" s="69">
         <v>942.84</v>
       </c>
-      <c r="M41" s="246"/>
-      <c r="N41" s="248"/>
+      <c r="M41" s="247"/>
+      <c r="N41" s="249"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -14489,29 +14532,29 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="233" t="s">
+      <c r="H53" s="234" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="234"/>
+      <c r="I53" s="235"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="235">
+      <c r="K53" s="236">
         <f>I51+L51</f>
         <v>104139.16999999998</v>
       </c>
-      <c r="L53" s="236"/>
-      <c r="M53" s="224">
+      <c r="L53" s="237"/>
+      <c r="M53" s="225">
         <f>N40+M40</f>
         <v>2044992.5</v>
       </c>
-      <c r="N53" s="225"/>
+      <c r="N53" s="226"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="237" t="s">
+      <c r="D54" s="238" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="237"/>
+      <c r="E54" s="238"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
         <v>2004605.33</v>
@@ -14522,22 +14565,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="238" t="s">
+      <c r="D55" s="239" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="238"/>
+      <c r="E55" s="239"/>
       <c r="F55" s="102">
         <v>-2026393.17</v>
       </c>
-      <c r="I55" s="239" t="s">
+      <c r="I55" s="240" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="240"/>
-      <c r="K55" s="241">
+      <c r="J55" s="241"/>
+      <c r="K55" s="242">
         <f>F57+F58+F59</f>
         <v>178711.56000000014</v>
       </c>
-      <c r="L55" s="242"/>
+      <c r="L55" s="243"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -14568,11 +14611,11 @@
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="226">
+      <c r="K57" s="227">
         <f>-C4</f>
         <v>-134848.89000000001</v>
       </c>
-      <c r="L57" s="227"/>
+      <c r="L57" s="228"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -14589,22 +14632,22 @@
       <c r="C59" s="120">
         <v>44507</v>
       </c>
-      <c r="D59" s="228" t="s">
+      <c r="D59" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="229"/>
+      <c r="E59" s="230"/>
       <c r="F59" s="121">
         <v>192529.4</v>
       </c>
-      <c r="I59" s="230" t="s">
+      <c r="I59" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="231"/>
-      <c r="K59" s="232">
+      <c r="J59" s="232"/>
+      <c r="K59" s="233">
         <f>K55+K57</f>
         <v>43862.670000000129</v>
       </c>
-      <c r="L59" s="232"/>
+      <c r="L59" s="233"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -14783,8 +14826,8 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A46" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15653,13 +15696,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="187">
+      <c r="A50" s="144">
         <v>44503</v>
       </c>
-      <c r="B50" s="185" t="s">
+      <c r="B50" s="142" t="s">
         <v>253</v>
       </c>
-      <c r="C50" s="186">
+      <c r="C50" s="79">
         <v>76941.100000000006</v>
       </c>
       <c r="D50" s="144"/>
@@ -15670,13 +15713,13 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="187">
+      <c r="A51" s="144">
         <v>44503</v>
       </c>
-      <c r="B51" s="185" t="s">
+      <c r="B51" s="142" t="s">
         <v>254</v>
       </c>
-      <c r="C51" s="186">
+      <c r="C51" s="79">
         <v>13212</v>
       </c>
       <c r="D51" s="144"/>
@@ -15693,99 +15736,99 @@
       <c r="B52" s="185" t="s">
         <v>255</v>
       </c>
-      <c r="C52" s="186">
-        <v>5106</v>
+      <c r="C52" s="79">
+        <v>0</v>
       </c>
       <c r="D52" s="144"/>
       <c r="E52" s="79"/>
       <c r="F52" s="145">
         <f t="shared" si="0"/>
-        <v>95259.1</v>
+        <v>90153.1</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="187">
+      <c r="A53" s="144">
         <v>44504</v>
       </c>
-      <c r="B53" s="185" t="s">
+      <c r="B53" s="142" t="s">
         <v>256</v>
       </c>
-      <c r="C53" s="186">
+      <c r="C53" s="79">
         <v>2750</v>
       </c>
       <c r="D53" s="144"/>
       <c r="E53" s="79"/>
       <c r="F53" s="145">
         <f t="shared" si="0"/>
-        <v>98009.1</v>
+        <v>92903.1</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="188">
+      <c r="A54" s="141">
         <v>44504</v>
       </c>
-      <c r="B54" s="185" t="s">
+      <c r="B54" s="142" t="s">
         <v>257</v>
       </c>
-      <c r="C54" s="186">
+      <c r="C54" s="79">
         <v>5694</v>
       </c>
       <c r="D54" s="144"/>
       <c r="E54" s="79"/>
       <c r="F54" s="145">
         <f t="shared" si="0"/>
-        <v>103703.1</v>
+        <v>98597.1</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="188">
+      <c r="A55" s="141">
         <v>44505</v>
       </c>
-      <c r="B55" s="185" t="s">
+      <c r="B55" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="C55" s="186">
+      <c r="C55" s="79">
         <v>97618</v>
       </c>
       <c r="D55" s="144"/>
       <c r="E55" s="79"/>
       <c r="F55" s="145">
         <f t="shared" si="0"/>
-        <v>201321.1</v>
+        <v>196215.1</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="188">
+      <c r="A56" s="141">
         <v>44505</v>
       </c>
-      <c r="B56" s="185" t="s">
+      <c r="B56" s="142" t="s">
         <v>259</v>
       </c>
-      <c r="C56" s="186">
+      <c r="C56" s="79">
         <v>6914</v>
       </c>
       <c r="D56" s="144"/>
       <c r="E56" s="79"/>
       <c r="F56" s="145">
         <f t="shared" si="0"/>
-        <v>208235.1</v>
+        <v>203129.1</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="187">
+      <c r="A57" s="144">
         <v>44506</v>
       </c>
-      <c r="B57" s="185" t="s">
+      <c r="B57" s="142" t="s">
         <v>260</v>
       </c>
-      <c r="C57" s="186">
+      <c r="C57" s="79">
         <v>96936.9</v>
       </c>
       <c r="D57" s="144"/>
       <c r="E57" s="79"/>
       <c r="F57" s="145">
         <f t="shared" si="0"/>
-        <v>305172</v>
+        <v>300066</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -15802,7 +15845,7 @@
       <c r="E58" s="79"/>
       <c r="F58" s="145">
         <f t="shared" si="0"/>
-        <v>311749.2</v>
+        <v>306643.20000000001</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -15815,11 +15858,15 @@
       <c r="C59" s="79">
         <v>606</v>
       </c>
-      <c r="D59" s="144"/>
-      <c r="E59" s="79"/>
+      <c r="D59" s="144">
+        <v>44512</v>
+      </c>
+      <c r="E59" s="79">
+        <v>307249.2</v>
+      </c>
       <c r="F59" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -15830,7 +15877,7 @@
       <c r="E60" s="79"/>
       <c r="F60" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -15841,7 +15888,7 @@
       <c r="E61" s="79"/>
       <c r="F61" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -15852,7 +15899,7 @@
       <c r="E62" s="79"/>
       <c r="F62" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15863,7 +15910,7 @@
       <c r="E63" s="79"/>
       <c r="F63" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15874,7 +15921,7 @@
       <c r="E64" s="79"/>
       <c r="F64" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15885,7 +15932,7 @@
       <c r="E65" s="79"/>
       <c r="F65" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15896,7 +15943,7 @@
       <c r="E66" s="79"/>
       <c r="F66" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15907,7 +15954,7 @@
       <c r="E67" s="79"/>
       <c r="F67" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15918,7 +15965,7 @@
       <c r="E68" s="79"/>
       <c r="F68" s="145">
         <f t="shared" si="0"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15929,7 +15976,7 @@
       <c r="E69" s="79"/>
       <c r="F69" s="145">
         <f t="shared" ref="F69:F97" si="1">F68+C69-E69</f>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15940,7 +15987,7 @@
       <c r="E70" s="79"/>
       <c r="F70" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15951,7 +15998,7 @@
       <c r="E71" s="79"/>
       <c r="F71" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15962,7 +16009,7 @@
       <c r="E72" s="79"/>
       <c r="F72" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15973,7 +16020,7 @@
       <c r="E73" s="79"/>
       <c r="F73" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15984,7 +16031,7 @@
       <c r="E74" s="79"/>
       <c r="F74" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -15995,7 +16042,7 @@
       <c r="E75" s="79"/>
       <c r="F75" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16006,7 +16053,7 @@
       <c r="E76" s="79"/>
       <c r="F76" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16017,7 +16064,7 @@
       <c r="E77" s="79"/>
       <c r="F77" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16028,7 +16075,7 @@
       <c r="E78" s="79"/>
       <c r="F78" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16039,7 +16086,7 @@
       <c r="E79" s="79"/>
       <c r="F79" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16050,7 +16097,7 @@
       <c r="E80" s="79"/>
       <c r="F80" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16061,7 +16108,7 @@
       <c r="E81" s="83"/>
       <c r="F81" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16072,7 +16119,7 @@
       <c r="E82" s="83"/>
       <c r="F82" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16083,7 +16130,7 @@
       <c r="E83" s="83"/>
       <c r="F83" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16094,7 +16141,7 @@
       <c r="E84" s="83"/>
       <c r="F84" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16105,7 +16152,7 @@
       <c r="E85" s="83"/>
       <c r="F85" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16116,7 +16163,7 @@
       <c r="E86" s="83"/>
       <c r="F86" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16127,7 +16174,7 @@
       <c r="E87" s="79"/>
       <c r="F87" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16138,7 +16185,7 @@
       <c r="E88" s="79"/>
       <c r="F88" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16149,7 +16196,7 @@
       <c r="E89" s="79"/>
       <c r="F89" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16160,7 +16207,7 @@
       <c r="E90" s="79"/>
       <c r="F90" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16171,7 +16218,7 @@
       <c r="E91" s="79"/>
       <c r="F91" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16182,7 +16229,7 @@
       <c r="E92" s="79"/>
       <c r="F92" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16193,7 +16240,7 @@
       <c r="E93" s="79"/>
       <c r="F93" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16204,7 +16251,7 @@
       <c r="E94" s="79"/>
       <c r="F94" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16215,7 +16262,7 @@
       <c r="E95" s="79"/>
       <c r="F95" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -16226,7 +16273,7 @@
       <c r="E96" s="79"/>
       <c r="F96" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -16239,23 +16286,23 @@
       <c r="E97" s="151"/>
       <c r="F97" s="145">
         <f t="shared" si="1"/>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B98" s="104"/>
       <c r="C98" s="3">
         <f>SUM(C3:C97)</f>
-        <v>2026393.17</v>
+        <v>2021287.17</v>
       </c>
       <c r="D98" s="103"/>
       <c r="E98" s="3">
         <f>SUM(E3:E97)</f>
-        <v>1714037.97</v>
+        <v>2021287.17</v>
       </c>
       <c r="F98" s="153">
         <f>F97</f>
-        <v>312355.20000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -16462,8 +16509,8 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16485,23 +16532,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="249"/>
-      <c r="C1" s="258" t="s">
+      <c r="B1" s="250"/>
+      <c r="C1" s="259" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
-      <c r="J1" s="259"/>
-      <c r="K1" s="259"/>
-      <c r="L1" s="259"/>
-      <c r="M1" s="259"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="260"/>
+      <c r="F1" s="260"/>
+      <c r="G1" s="260"/>
+      <c r="H1" s="260"/>
+      <c r="I1" s="260"/>
+      <c r="J1" s="260"/>
+      <c r="K1" s="260"/>
+      <c r="L1" s="260"/>
+      <c r="M1" s="260"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="250"/>
+      <c r="B2" s="251"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -16511,17 +16558,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="251" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="252"/>
+      <c r="B3" s="252" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="253"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="253" t="s">
+      <c r="H3" s="254" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="253"/>
+      <c r="I3" s="254"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -16537,14 +16584,14 @@
       <c r="D4" s="16">
         <v>44507</v>
       </c>
-      <c r="E4" s="254" t="s">
+      <c r="E4" s="255" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="255"/>
-      <c r="H4" s="256" t="s">
+      <c r="F4" s="256"/>
+      <c r="H4" s="257" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="257"/>
+      <c r="I4" s="258"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -16554,10 +16601,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="243" t="s">
+      <c r="P4" s="244" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="244"/>
+      <c r="Q4" s="245"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -17239,33 +17286,40 @@
       <c r="B20" s="21">
         <v>44523</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="22">
+        <v>0</v>
+      </c>
       <c r="D20" s="31"/>
       <c r="E20" s="24">
         <v>44523</v>
       </c>
-      <c r="F20" s="25"/>
+      <c r="F20" s="25">
+        <v>38803</v>
+      </c>
       <c r="G20" s="26"/>
       <c r="H20" s="32">
         <v>44523</v>
       </c>
-      <c r="I20" s="28"/>
+      <c r="I20" s="28">
+        <v>15</v>
+      </c>
       <c r="J20" s="33"/>
       <c r="K20" s="50"/>
       <c r="L20" s="43"/>
       <c r="M20" s="138">
-        <v>0</v>
+        <f>20000+18790</f>
+        <v>38790</v>
       </c>
       <c r="N20" s="30">
         <v>0</v>
       </c>
       <c r="P20" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38805</v>
       </c>
       <c r="Q20" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R20" s="26"/>
     </row>
@@ -17274,33 +17328,42 @@
       <c r="B21" s="21">
         <v>44524</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="22">
+        <v>4880</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>267</v>
+      </c>
       <c r="E21" s="24">
         <v>44524</v>
       </c>
-      <c r="F21" s="25"/>
+      <c r="F21" s="25">
+        <v>41176</v>
+      </c>
       <c r="G21" s="26"/>
       <c r="H21" s="32">
         <v>44524</v>
       </c>
-      <c r="I21" s="28"/>
+      <c r="I21" s="28">
+        <v>35</v>
+      </c>
       <c r="J21" s="33"/>
       <c r="K21" s="177"/>
       <c r="L21" s="43"/>
       <c r="M21" s="138">
-        <v>0</v>
+        <f>20000+16260</f>
+        <v>36260</v>
       </c>
       <c r="N21" s="30">
         <v>0</v>
       </c>
       <c r="P21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>41175</v>
+      </c>
+      <c r="Q21" s="217">
+        <f t="shared" si="1"/>
+        <v>-1</v>
       </c>
       <c r="R21" s="26"/>
     </row>
@@ -17309,32 +17372,40 @@
       <c r="B22" s="21">
         <v>44525</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="22">
+        <v>0</v>
+      </c>
       <c r="D22" s="31"/>
       <c r="E22" s="24">
         <v>44525</v>
       </c>
-      <c r="F22" s="25"/>
+      <c r="F22" s="25">
+        <v>62185</v>
+      </c>
       <c r="G22" s="26"/>
       <c r="H22" s="32">
         <v>44525</v>
       </c>
-      <c r="I22" s="28"/>
+      <c r="I22" s="28">
+        <v>0</v>
+      </c>
       <c r="J22" s="33"/>
       <c r="K22" s="51"/>
       <c r="L22" s="52"/>
-      <c r="M22" s="138">
-        <v>0</v>
+      <c r="M22" s="224">
+        <f>25000</f>
+        <v>25000</v>
       </c>
       <c r="N22" s="30">
         <v>0</v>
       </c>
       <c r="P22" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>4</v>
+        <v>25000</v>
+      </c>
+      <c r="Q22" s="136">
+        <f t="shared" si="1"/>
+        <v>-37185</v>
       </c>
       <c r="R22" s="26"/>
     </row>
@@ -17367,7 +17438,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="Q23" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17402,7 +17473,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="Q24" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17437,7 +17508,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="Q25" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17475,7 +17546,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="Q26" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17510,7 +17581,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="9">
+      <c r="Q27" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17545,7 +17616,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="Q28" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17580,7 +17651,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="9">
+      <c r="Q29" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17904,21 +17975,21 @@
       <c r="J40" s="67"/>
       <c r="K40" s="82"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="245">
+      <c r="M40" s="246">
         <f>SUM(M5:M39)</f>
-        <v>906958</v>
-      </c>
-      <c r="N40" s="247">
+        <v>1007008</v>
+      </c>
+      <c r="N40" s="248">
         <f>SUM(N5:N39)</f>
         <v>20583</v>
       </c>
       <c r="P40" s="83">
         <f>SUM(P5:P39)</f>
-        <v>996571.34</v>
+        <v>1101551.3399999999</v>
       </c>
       <c r="Q40" s="222">
         <f>SUM(Q5:Q38)</f>
-        <v>7999.3399999999965</v>
+        <v>-29184.660000000003</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17934,8 +18005,8 @@
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="69"/>
-      <c r="M41" s="246"/>
-      <c r="N41" s="248"/>
+      <c r="M41" s="247"/>
+      <c r="N41" s="249"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -18108,7 +18179,7 @@
       </c>
       <c r="C51" s="93">
         <f>SUM(C5:C50)</f>
-        <v>37884</v>
+        <v>42764</v>
       </c>
       <c r="D51" s="94"/>
       <c r="E51" s="95" t="s">
@@ -18116,7 +18187,7 @@
       </c>
       <c r="F51" s="96">
         <f>SUM(F5:F50)</f>
-        <v>988572</v>
+        <v>1130736</v>
       </c>
       <c r="G51" s="94"/>
       <c r="H51" s="97" t="s">
@@ -18124,7 +18195,7 @@
       </c>
       <c r="I51" s="98">
         <f>SUM(I5:I50)</f>
-        <v>5705</v>
+        <v>5755</v>
       </c>
       <c r="J51" s="99"/>
       <c r="K51" s="100" t="s">
@@ -18150,32 +18221,32 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="233" t="s">
+      <c r="H53" s="234" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="234"/>
+      <c r="I53" s="235"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="235">
+      <c r="K53" s="236">
         <f>I51+L51</f>
-        <v>31146.34</v>
-      </c>
-      <c r="L53" s="236"/>
-      <c r="M53" s="224">
+        <v>31196.34</v>
+      </c>
+      <c r="L53" s="237"/>
+      <c r="M53" s="225">
         <f>N40+M40</f>
-        <v>927541</v>
-      </c>
-      <c r="N53" s="225"/>
+        <v>1027591</v>
+      </c>
+      <c r="N53" s="226"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="237" t="s">
+      <c r="D54" s="238" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="237"/>
+      <c r="E54" s="238"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
-        <v>919541.66</v>
+        <v>1056775.6599999999</v>
       </c>
       <c r="I54" s="108"/>
       <c r="J54" s="109"/>
@@ -18183,22 +18254,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="238" t="s">
+      <c r="D55" s="239" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="238"/>
+      <c r="E55" s="239"/>
       <c r="F55" s="102">
         <v>0</v>
       </c>
-      <c r="I55" s="239" t="s">
+      <c r="I55" s="240" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="240"/>
-      <c r="K55" s="241">
+      <c r="J55" s="241"/>
+      <c r="K55" s="242">
         <f>F57+F58+F59</f>
-        <v>919541.66</v>
-      </c>
-      <c r="L55" s="242"/>
+        <v>1056775.6599999999</v>
+      </c>
+      <c r="L55" s="243"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -18222,18 +18293,18 @@
       </c>
       <c r="F57" s="102">
         <f>SUM(F54:F56)</f>
-        <v>919541.66</v>
+        <v>1056775.6599999999</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="226">
+      <c r="K57" s="227">
         <f>-C4</f>
         <v>-192529.4</v>
       </c>
-      <c r="L57" s="227"/>
+      <c r="L57" s="228"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -18248,22 +18319,22 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="120"/>
-      <c r="D59" s="228" t="s">
+      <c r="D59" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="229"/>
+      <c r="E59" s="230"/>
       <c r="F59" s="121">
         <v>0</v>
       </c>
-      <c r="I59" s="230" t="s">
+      <c r="I59" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="231"/>
-      <c r="K59" s="232">
+      <c r="J59" s="232"/>
+      <c r="K59" s="233">
         <f>K55+K57</f>
-        <v>727012.26</v>
-      </c>
-      <c r="L59" s="232"/>
+        <v>864246.25999999989</v>
+      </c>
+      <c r="L59" s="233"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -18442,8 +18513,8 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18489,159 +18560,251 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="141"/>
-      <c r="B3" s="179"/>
-      <c r="C3" s="79"/>
+      <c r="A3" s="141">
+        <v>44508</v>
+      </c>
+      <c r="B3" s="179" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="79">
+        <v>21631.48</v>
+      </c>
       <c r="D3" s="203"/>
       <c r="E3" s="79"/>
       <c r="F3" s="143">
         <f>C3-E3</f>
-        <v>0</v>
+        <v>21631.48</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="141"/>
-      <c r="B4" s="179"/>
-      <c r="C4" s="79"/>
+      <c r="A4" s="141">
+        <v>44510</v>
+      </c>
+      <c r="B4" s="179" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="79">
+        <v>95563.8</v>
+      </c>
       <c r="D4" s="203"/>
       <c r="E4" s="79"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
-        <v>0</v>
+        <v>117195.28</v>
       </c>
       <c r="G4" s="146"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="141"/>
-      <c r="B5" s="179"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="79"/>
+      <c r="A5" s="141">
+        <v>44510</v>
+      </c>
+      <c r="B5" s="179" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="79">
+        <v>23572.27</v>
+      </c>
+      <c r="D5" s="221">
+        <v>44481</v>
+      </c>
+      <c r="E5" s="79">
+        <v>140767.54999999999</v>
+      </c>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="141"/>
-      <c r="B6" s="179"/>
-      <c r="C6" s="79"/>
+      <c r="A6" s="141">
+        <v>44510</v>
+      </c>
+      <c r="B6" s="179" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" s="79">
+        <v>504</v>
+      </c>
       <c r="D6" s="203"/>
       <c r="E6" s="79"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="141"/>
-      <c r="B7" s="179"/>
-      <c r="C7" s="79"/>
+      <c r="A7" s="141">
+        <v>44511</v>
+      </c>
+      <c r="B7" s="179" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="79">
+        <v>40140.839999999997</v>
+      </c>
       <c r="D7" s="203"/>
       <c r="E7" s="79"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40644.839999999997</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="141"/>
-      <c r="B8" s="179"/>
-      <c r="C8" s="79"/>
+      <c r="A8" s="141">
+        <v>44513</v>
+      </c>
+      <c r="B8" s="179" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="79">
+        <v>123754.4</v>
+      </c>
       <c r="D8" s="203"/>
       <c r="E8" s="79"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>164399.24</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="141"/>
-      <c r="B9" s="179"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="141">
+        <v>44513</v>
+      </c>
+      <c r="B9" s="179" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="79">
+        <v>27945.79</v>
+      </c>
       <c r="D9" s="203"/>
       <c r="E9" s="79"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>192345.03</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="141"/>
-      <c r="B10" s="179"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="141">
+        <v>44513</v>
+      </c>
+      <c r="B10" s="179" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="79">
+        <v>4108</v>
+      </c>
       <c r="D10" s="203"/>
       <c r="E10" s="79"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>196453.03</v>
       </c>
       <c r="G10" s="146"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="141"/>
-      <c r="B11" s="142"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="141">
+        <v>44513</v>
+      </c>
+      <c r="B11" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="79">
+        <v>20972</v>
+      </c>
       <c r="D11" s="144"/>
       <c r="E11" s="79"/>
       <c r="F11" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>217425.03</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="144"/>
-      <c r="B12" s="142"/>
-      <c r="C12" s="79"/>
+      <c r="A12" s="144">
+        <v>44515</v>
+      </c>
+      <c r="B12" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="79">
+        <v>41874.6</v>
+      </c>
       <c r="D12" s="144"/>
       <c r="E12" s="79"/>
       <c r="F12" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>259299.63</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="144"/>
-      <c r="B13" s="142"/>
-      <c r="C13" s="79"/>
+      <c r="A13" s="144">
+        <v>15111</v>
+      </c>
+      <c r="B13" s="142" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="79">
+        <v>10480.799999999999</v>
+      </c>
       <c r="D13" s="144"/>
       <c r="E13" s="79"/>
       <c r="F13" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>269780.43</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="144"/>
-      <c r="B14" s="142"/>
-      <c r="C14" s="79"/>
+      <c r="A14" s="144">
+        <v>44516</v>
+      </c>
+      <c r="B14" s="142" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="79">
+        <v>3918.4</v>
+      </c>
       <c r="D14" s="144"/>
       <c r="E14" s="79"/>
       <c r="F14" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>273698.83</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
-      <c r="B15" s="142"/>
-      <c r="C15" s="79"/>
+      <c r="A15" s="144">
+        <v>44516</v>
+      </c>
+      <c r="B15" s="142" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="79">
+        <v>107092.1</v>
+      </c>
       <c r="D15" s="144"/>
       <c r="E15" s="79"/>
       <c r="F15" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>380790.93000000005</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="144"/>
-      <c r="B16" s="142"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="79"/>
+      <c r="A16" s="144">
+        <v>44517</v>
+      </c>
+      <c r="B16" s="142" t="s">
+        <v>292</v>
+      </c>
+      <c r="C16" s="79">
+        <v>84186.4</v>
+      </c>
+      <c r="D16" s="144">
+        <v>44519</v>
+      </c>
+      <c r="E16" s="79">
+        <v>385896.93</v>
+      </c>
       <c r="F16" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18652,7 +18815,7 @@
       <c r="E17" s="79"/>
       <c r="F17" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18663,7 +18826,7 @@
       <c r="E18" s="79"/>
       <c r="F18" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18674,7 +18837,7 @@
       <c r="E19" s="79"/>
       <c r="F19" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18685,7 +18848,7 @@
       <c r="E20" s="79"/>
       <c r="F20" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18696,7 +18859,7 @@
       <c r="E21" s="79"/>
       <c r="F21" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -18707,7 +18870,7 @@
       <c r="E22" s="79"/>
       <c r="F22" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
       <c r="G22" s="146"/>
     </row>
@@ -18719,7 +18882,7 @@
       <c r="E23" s="79"/>
       <c r="F23" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18730,7 +18893,7 @@
       <c r="E24" s="79"/>
       <c r="F24" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18741,7 +18904,7 @@
       <c r="E25" s="79"/>
       <c r="F25" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18752,7 +18915,7 @@
       <c r="E26" s="79"/>
       <c r="F26" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18763,7 +18926,7 @@
       <c r="E27" s="79"/>
       <c r="F27" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18774,7 +18937,7 @@
       <c r="E28" s="79"/>
       <c r="F28" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18785,7 +18948,7 @@
       <c r="E29" s="79"/>
       <c r="F29" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -18796,7 +18959,7 @@
       <c r="E30" s="79"/>
       <c r="F30" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
       <c r="G30" s="146"/>
     </row>
@@ -18808,7 +18971,7 @@
       <c r="E31" s="79"/>
       <c r="F31" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -18819,7 +18982,7 @@
       <c r="E32" s="79"/>
       <c r="F32" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18830,7 +18993,7 @@
       <c r="E33" s="79"/>
       <c r="F33" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18841,7 +19004,7 @@
       <c r="E34" s="79"/>
       <c r="F34" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18852,7 +19015,7 @@
       <c r="E35" s="79"/>
       <c r="F35" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18863,7 +19026,7 @@
       <c r="E36" s="79"/>
       <c r="F36" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18874,7 +19037,7 @@
       <c r="E37" s="79"/>
       <c r="F37" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18885,7 +19048,7 @@
       <c r="E38" s="79"/>
       <c r="F38" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18896,7 +19059,7 @@
       <c r="E39" s="79"/>
       <c r="F39" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18907,7 +19070,7 @@
       <c r="E40" s="79"/>
       <c r="F40" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18918,7 +19081,7 @@
       <c r="E41" s="79"/>
       <c r="F41" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18929,7 +19092,7 @@
       <c r="E42" s="79"/>
       <c r="F42" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18940,7 +19103,7 @@
       <c r="E43" s="79"/>
       <c r="F43" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18951,7 +19114,7 @@
       <c r="E44" s="79"/>
       <c r="F44" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18962,7 +19125,7 @@
       <c r="E45" s="79"/>
       <c r="F45" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18973,7 +19136,7 @@
       <c r="E46" s="79"/>
       <c r="F46" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18984,7 +19147,7 @@
       <c r="E47" s="79"/>
       <c r="F47" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18995,7 +19158,7 @@
       <c r="E48" s="79"/>
       <c r="F48" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19006,7 +19169,7 @@
       <c r="E49" s="79"/>
       <c r="F49" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19017,7 +19180,7 @@
       <c r="E50" s="79"/>
       <c r="F50" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19028,7 +19191,7 @@
       <c r="E51" s="79"/>
       <c r="F51" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19039,7 +19202,7 @@
       <c r="E52" s="79"/>
       <c r="F52" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19050,7 +19213,7 @@
       <c r="E53" s="79"/>
       <c r="F53" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19061,7 +19224,7 @@
       <c r="E54" s="79"/>
       <c r="F54" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19072,7 +19235,7 @@
       <c r="E55" s="79"/>
       <c r="F55" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19083,7 +19246,7 @@
       <c r="E56" s="79"/>
       <c r="F56" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19094,7 +19257,7 @@
       <c r="E57" s="79"/>
       <c r="F57" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19105,7 +19268,7 @@
       <c r="E58" s="79"/>
       <c r="F58" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19116,7 +19279,7 @@
       <c r="E59" s="79"/>
       <c r="F59" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19127,7 +19290,7 @@
       <c r="E60" s="79"/>
       <c r="F60" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19138,7 +19301,7 @@
       <c r="E61" s="79"/>
       <c r="F61" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -19149,7 +19312,7 @@
       <c r="E62" s="79"/>
       <c r="F62" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19160,7 +19323,7 @@
       <c r="E63" s="79"/>
       <c r="F63" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19171,7 +19334,7 @@
       <c r="E64" s="79"/>
       <c r="F64" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19182,7 +19345,7 @@
       <c r="E65" s="79"/>
       <c r="F65" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19193,7 +19356,7 @@
       <c r="E66" s="79"/>
       <c r="F66" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19204,7 +19367,7 @@
       <c r="E67" s="79"/>
       <c r="F67" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19215,7 +19378,7 @@
       <c r="E68" s="79"/>
       <c r="F68" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19226,7 +19389,7 @@
       <c r="E69" s="79"/>
       <c r="F69" s="145">
         <f t="shared" ref="F69:F97" si="1">F68+C69-E69</f>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19237,7 +19400,7 @@
       <c r="E70" s="79"/>
       <c r="F70" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19248,7 +19411,7 @@
       <c r="E71" s="79"/>
       <c r="F71" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19259,7 +19422,7 @@
       <c r="E72" s="79"/>
       <c r="F72" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19270,7 +19433,7 @@
       <c r="E73" s="79"/>
       <c r="F73" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19281,7 +19444,7 @@
       <c r="E74" s="79"/>
       <c r="F74" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19292,7 +19455,7 @@
       <c r="E75" s="79"/>
       <c r="F75" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19303,7 +19466,7 @@
       <c r="E76" s="79"/>
       <c r="F76" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19314,7 +19477,7 @@
       <c r="E77" s="79"/>
       <c r="F77" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19325,7 +19488,7 @@
       <c r="E78" s="79"/>
       <c r="F78" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19336,7 +19499,7 @@
       <c r="E79" s="79"/>
       <c r="F79" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19347,7 +19510,7 @@
       <c r="E80" s="79"/>
       <c r="F80" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19358,7 +19521,7 @@
       <c r="E81" s="83"/>
       <c r="F81" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19369,7 +19532,7 @@
       <c r="E82" s="83"/>
       <c r="F82" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19380,7 +19543,7 @@
       <c r="E83" s="83"/>
       <c r="F83" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19391,7 +19554,7 @@
       <c r="E84" s="83"/>
       <c r="F84" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19402,7 +19565,7 @@
       <c r="E85" s="83"/>
       <c r="F85" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19413,7 +19576,7 @@
       <c r="E86" s="83"/>
       <c r="F86" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19424,7 +19587,7 @@
       <c r="E87" s="79"/>
       <c r="F87" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19435,7 +19598,7 @@
       <c r="E88" s="79"/>
       <c r="F88" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19446,7 +19609,7 @@
       <c r="E89" s="79"/>
       <c r="F89" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19457,7 +19620,7 @@
       <c r="E90" s="79"/>
       <c r="F90" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19468,7 +19631,7 @@
       <c r="E91" s="79"/>
       <c r="F91" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19479,7 +19642,7 @@
       <c r="E92" s="79"/>
       <c r="F92" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19490,7 +19653,7 @@
       <c r="E93" s="79"/>
       <c r="F93" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19501,7 +19664,7 @@
       <c r="E94" s="79"/>
       <c r="F94" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19512,7 +19675,7 @@
       <c r="E95" s="79"/>
       <c r="F95" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -19523,7 +19686,7 @@
       <c r="E96" s="79"/>
       <c r="F96" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -19536,23 +19699,23 @@
       <c r="E97" s="151"/>
       <c r="F97" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B98" s="104"/>
       <c r="C98" s="3">
         <f>SUM(C3:C97)</f>
-        <v>0</v>
+        <v>605744.88</v>
       </c>
       <c r="D98" s="103"/>
       <c r="E98" s="3">
         <f>SUM(E3:E97)</f>
-        <v>0</v>
+        <v>526664.48</v>
       </c>
       <c r="F98" s="153">
         <f>F97</f>
-        <v>0</v>
+        <v>79080.400000000081</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -19749,6 +19912,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>